<commit_message>
Results simulations 2024 with low interest rate for nuclear
</commit_message>
<xml_diff>
--- a/rawResults/Summary.xlsx
+++ b/rawResults/Summary.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AF4"/>
+  <dimension ref="A1:AF7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -913,6 +913,324 @@
         </is>
       </c>
     </row>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>273331505167.4862</v>
+      </c>
+      <c r="B5" t="n">
+        <v>47916585452.44899</v>
+      </c>
+      <c r="C5" t="n">
+        <v>3231141846.958039</v>
+      </c>
+      <c r="D5" t="n">
+        <v>216993108108.0792</v>
+      </c>
+      <c r="E5" t="n">
+        <v>5190669759.999999</v>
+      </c>
+      <c r="F5" t="n">
+        <v>264909693560.5281</v>
+      </c>
+      <c r="G5" t="n">
+        <v>8421811606.958038</v>
+      </c>
+      <c r="H5" t="n">
+        <v>0</v>
+      </c>
+      <c r="I5" t="n">
+        <v>0</v>
+      </c>
+      <c r="J5" t="n">
+        <v>0</v>
+      </c>
+      <c r="K5" t="n">
+        <v>0</v>
+      </c>
+      <c r="L5" t="n">
+        <v>0</v>
+      </c>
+      <c r="M5" t="n">
+        <v>273331505167.4862</v>
+      </c>
+      <c r="N5" t="n">
+        <v>0</v>
+      </c>
+      <c r="O5" t="n">
+        <v>0</v>
+      </c>
+      <c r="P5" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q5" t="n">
+        <v>0</v>
+      </c>
+      <c r="R5" t="n">
+        <v>0</v>
+      </c>
+      <c r="S5" t="n">
+        <v>0</v>
+      </c>
+      <c r="T5" t="n">
+        <v>0</v>
+      </c>
+      <c r="U5" t="n">
+        <v>0</v>
+      </c>
+      <c r="V5" t="n">
+        <v>36003.24399995804</v>
+      </c>
+      <c r="W5" t="n">
+        <v>263288439384.9565</v>
+      </c>
+      <c r="X5" t="n">
+        <v>273331505167.4862</v>
+      </c>
+      <c r="Y5" t="n">
+        <v>10043065782.52972</v>
+      </c>
+      <c r="Z5" t="inlineStr">
+        <is>
+          <t>maxTimeLimit</t>
+        </is>
+      </c>
+      <c r="AA5" t="inlineStr">
+        <is>
+          <t>costs_emissionlimit</t>
+        </is>
+      </c>
+      <c r="AB5" t="n">
+        <v>-1</v>
+      </c>
+      <c r="AC5" t="n">
+        <v>-1</v>
+      </c>
+      <c r="AD5" t="n">
+        <v>1</v>
+      </c>
+      <c r="AE5" t="inlineStr">
+        <is>
+          <t>GreenFieldHydro_Island</t>
+        </is>
+      </c>
+      <c r="AF5" t="inlineStr">
+        <is>
+          <t>rawResults\20251120145249_GreenFieldHydro_Island-1</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="n">
+        <v>263438979519.0895</v>
+      </c>
+      <c r="B6" t="n">
+        <v>35900523400.00355</v>
+      </c>
+      <c r="C6" t="n">
+        <v>5134357388.413489</v>
+      </c>
+      <c r="D6" t="n">
+        <v>215352264839.8636</v>
+      </c>
+      <c r="E6" t="n">
+        <v>7051833890.80888</v>
+      </c>
+      <c r="F6" t="n">
+        <v>251252788239.8671</v>
+      </c>
+      <c r="G6" t="n">
+        <v>12186191279.22237</v>
+      </c>
+      <c r="H6" t="n">
+        <v>0</v>
+      </c>
+      <c r="I6" t="n">
+        <v>0</v>
+      </c>
+      <c r="J6" t="n">
+        <v>0</v>
+      </c>
+      <c r="K6" t="n">
+        <v>0</v>
+      </c>
+      <c r="L6" t="n">
+        <v>0</v>
+      </c>
+      <c r="M6" t="n">
+        <v>263438979519.0895</v>
+      </c>
+      <c r="N6" t="n">
+        <v>0</v>
+      </c>
+      <c r="O6" t="n">
+        <v>0</v>
+      </c>
+      <c r="P6" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q6" t="n">
+        <v>0</v>
+      </c>
+      <c r="R6" t="n">
+        <v>0</v>
+      </c>
+      <c r="S6" t="n">
+        <v>0</v>
+      </c>
+      <c r="T6" t="n">
+        <v>0</v>
+      </c>
+      <c r="U6" t="n">
+        <v>0</v>
+      </c>
+      <c r="V6" t="n">
+        <v>21621.41000008583</v>
+      </c>
+      <c r="W6" t="n">
+        <v>263438977169.5732</v>
+      </c>
+      <c r="X6" t="n">
+        <v>263438979519.0895</v>
+      </c>
+      <c r="Y6" t="n">
+        <v>2349.516296386719</v>
+      </c>
+      <c r="Z6" t="inlineStr">
+        <is>
+          <t>optimal</t>
+        </is>
+      </c>
+      <c r="AA6" t="inlineStr">
+        <is>
+          <t>costs_emissionlimit</t>
+        </is>
+      </c>
+      <c r="AB6" t="n">
+        <v>-1</v>
+      </c>
+      <c r="AC6" t="n">
+        <v>-1</v>
+      </c>
+      <c r="AD6" t="n">
+        <v>1</v>
+      </c>
+      <c r="AE6" t="inlineStr">
+        <is>
+          <t>GreenFieldHydro_Island</t>
+        </is>
+      </c>
+      <c r="AF6" t="inlineStr">
+        <is>
+          <t>rawResults\20251121161221_GreenFieldHydro_Island-1</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="n">
+        <v>230085772776.3448</v>
+      </c>
+      <c r="B7" t="n">
+        <v>13313796935.41874</v>
+      </c>
+      <c r="C7" t="n">
+        <v>0</v>
+      </c>
+      <c r="D7" t="n">
+        <v>214741056080.9261</v>
+      </c>
+      <c r="E7" t="n">
+        <v>2030919760</v>
+      </c>
+      <c r="F7" t="n">
+        <v>228054853016.3448</v>
+      </c>
+      <c r="G7" t="n">
+        <v>2030919760</v>
+      </c>
+      <c r="H7" t="n">
+        <v>0</v>
+      </c>
+      <c r="I7" t="n">
+        <v>0</v>
+      </c>
+      <c r="J7" t="n">
+        <v>0</v>
+      </c>
+      <c r="K7" t="n">
+        <v>0</v>
+      </c>
+      <c r="L7" t="n">
+        <v>0</v>
+      </c>
+      <c r="M7" t="n">
+        <v>230085772776.3448</v>
+      </c>
+      <c r="N7" t="n">
+        <v>0</v>
+      </c>
+      <c r="O7" t="n">
+        <v>0</v>
+      </c>
+      <c r="P7" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q7" t="n">
+        <v>0</v>
+      </c>
+      <c r="R7" t="n">
+        <v>0</v>
+      </c>
+      <c r="S7" t="n">
+        <v>0</v>
+      </c>
+      <c r="T7" t="n">
+        <v>0</v>
+      </c>
+      <c r="U7" t="n">
+        <v>0</v>
+      </c>
+      <c r="V7" t="n">
+        <v>1915.94100022316</v>
+      </c>
+      <c r="W7" t="n">
+        <v>230085772185.4905</v>
+      </c>
+      <c r="X7" t="n">
+        <v>230085772776.3448</v>
+      </c>
+      <c r="Y7" t="n">
+        <v>590.8543395996094</v>
+      </c>
+      <c r="Z7" t="inlineStr">
+        <is>
+          <t>optimal</t>
+        </is>
+      </c>
+      <c r="AA7" t="inlineStr">
+        <is>
+          <t>costs_emissionlimit</t>
+        </is>
+      </c>
+      <c r="AB7" t="n">
+        <v>-1</v>
+      </c>
+      <c r="AC7" t="n">
+        <v>-1</v>
+      </c>
+      <c r="AD7" t="n">
+        <v>1</v>
+      </c>
+      <c r="AE7" t="inlineStr">
+        <is>
+          <t>GreenFieldHydro_Island</t>
+        </is>
+      </c>
+      <c r="AF7" t="inlineStr">
+        <is>
+          <t>rawResults\20251124112706_GreenFieldHydro_Island-1</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Results simulations 2040 with low interest rate for nuclear
</commit_message>
<xml_diff>
--- a/rawResults/Summary.xlsx
+++ b/rawResults/Summary.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AF7"/>
+  <dimension ref="A1:AF8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1231,6 +1231,112 @@
         </is>
       </c>
     </row>
+    <row r="8">
+      <c r="A8" t="n">
+        <v>230085772776.3445</v>
+      </c>
+      <c r="B8" t="n">
+        <v>13313796935.41874</v>
+      </c>
+      <c r="C8" t="n">
+        <v>0</v>
+      </c>
+      <c r="D8" t="n">
+        <v>214741056080.9258</v>
+      </c>
+      <c r="E8" t="n">
+        <v>2030919760</v>
+      </c>
+      <c r="F8" t="n">
+        <v>228054853016.3445</v>
+      </c>
+      <c r="G8" t="n">
+        <v>2030919760</v>
+      </c>
+      <c r="H8" t="n">
+        <v>0</v>
+      </c>
+      <c r="I8" t="n">
+        <v>0</v>
+      </c>
+      <c r="J8" t="n">
+        <v>0</v>
+      </c>
+      <c r="K8" t="n">
+        <v>0</v>
+      </c>
+      <c r="L8" t="n">
+        <v>0</v>
+      </c>
+      <c r="M8" t="n">
+        <v>230085772776.3445</v>
+      </c>
+      <c r="N8" t="n">
+        <v>0</v>
+      </c>
+      <c r="O8" t="n">
+        <v>0</v>
+      </c>
+      <c r="P8" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q8" t="n">
+        <v>0</v>
+      </c>
+      <c r="R8" t="n">
+        <v>0</v>
+      </c>
+      <c r="S8" t="n">
+        <v>0</v>
+      </c>
+      <c r="T8" t="n">
+        <v>0</v>
+      </c>
+      <c r="U8" t="n">
+        <v>0</v>
+      </c>
+      <c r="V8" t="n">
+        <v>1827.349999904633</v>
+      </c>
+      <c r="W8" t="n">
+        <v>230085772185.4904</v>
+      </c>
+      <c r="X8" t="n">
+        <v>230085772776.3445</v>
+      </c>
+      <c r="Y8" t="n">
+        <v>590.8540649414062</v>
+      </c>
+      <c r="Z8" t="inlineStr">
+        <is>
+          <t>optimal</t>
+        </is>
+      </c>
+      <c r="AA8" t="inlineStr">
+        <is>
+          <t>costs_emissionlimit</t>
+        </is>
+      </c>
+      <c r="AB8" t="n">
+        <v>-1</v>
+      </c>
+      <c r="AC8" t="n">
+        <v>-1</v>
+      </c>
+      <c r="AD8" t="n">
+        <v>1</v>
+      </c>
+      <c r="AE8" t="inlineStr">
+        <is>
+          <t>GreenFieldHydro_Island_2040</t>
+        </is>
+      </c>
+      <c r="AF8" t="inlineStr">
+        <is>
+          <t>rawResults\20251124152705_GreenFieldHydro_Island_2040-1</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Fixed bug on the units of measure of the hydro inflows (GWh to MWh)
</commit_message>
<xml_diff>
--- a/rawResults/Summary.xlsx
+++ b/rawResults/Summary.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AF8"/>
+  <dimension ref="A1:AF10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1337,6 +1337,218 @@
         </is>
       </c>
     </row>
+    <row r="9">
+      <c r="A9" t="n">
+        <v>185851326104.2434</v>
+      </c>
+      <c r="B9" t="n">
+        <v>153358627530.0663</v>
+      </c>
+      <c r="C9" t="n">
+        <v>0</v>
+      </c>
+      <c r="D9" t="n">
+        <v>30461778814.17702</v>
+      </c>
+      <c r="E9" t="n">
+        <v>2030919760</v>
+      </c>
+      <c r="F9" t="n">
+        <v>183820406344.2434</v>
+      </c>
+      <c r="G9" t="n">
+        <v>2030919760</v>
+      </c>
+      <c r="H9" t="n">
+        <v>0</v>
+      </c>
+      <c r="I9" t="n">
+        <v>0</v>
+      </c>
+      <c r="J9" t="n">
+        <v>0</v>
+      </c>
+      <c r="K9" t="n">
+        <v>0</v>
+      </c>
+      <c r="L9" t="n">
+        <v>0</v>
+      </c>
+      <c r="M9" t="n">
+        <v>185851326104.2434</v>
+      </c>
+      <c r="N9" t="n">
+        <v>0</v>
+      </c>
+      <c r="O9" t="n">
+        <v>0</v>
+      </c>
+      <c r="P9" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q9" t="n">
+        <v>0</v>
+      </c>
+      <c r="R9" t="n">
+        <v>0</v>
+      </c>
+      <c r="S9" t="n">
+        <v>0</v>
+      </c>
+      <c r="T9" t="n">
+        <v>0</v>
+      </c>
+      <c r="U9" t="n">
+        <v>0</v>
+      </c>
+      <c r="V9" t="n">
+        <v>763.8449997901917</v>
+      </c>
+      <c r="W9" t="n">
+        <v>185851309924.4102</v>
+      </c>
+      <c r="X9" t="n">
+        <v>185851326104.2434</v>
+      </c>
+      <c r="Y9" t="n">
+        <v>16179.83316040039</v>
+      </c>
+      <c r="Z9" t="inlineStr">
+        <is>
+          <t>optimal</t>
+        </is>
+      </c>
+      <c r="AA9" t="inlineStr">
+        <is>
+          <t>costs_emissionlimit</t>
+        </is>
+      </c>
+      <c r="AB9" t="n">
+        <v>-1</v>
+      </c>
+      <c r="AC9" t="n">
+        <v>-1</v>
+      </c>
+      <c r="AD9" t="n">
+        <v>1</v>
+      </c>
+      <c r="AE9" t="inlineStr">
+        <is>
+          <t>GreenFieldHydro_Island_2040</t>
+        </is>
+      </c>
+      <c r="AF9" t="inlineStr">
+        <is>
+          <t>rawResults\20260203120741_GreenFieldHydro_Island_2040-1</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="n">
+        <v>168992919929.3019</v>
+      </c>
+      <c r="B10" t="n">
+        <v>143754608803.2541</v>
+      </c>
+      <c r="C10" t="n">
+        <v>0</v>
+      </c>
+      <c r="D10" t="n">
+        <v>27814901844.26778</v>
+      </c>
+      <c r="E10" t="n">
+        <v>2030919760</v>
+      </c>
+      <c r="F10" t="n">
+        <v>171569510647.5219</v>
+      </c>
+      <c r="G10" t="n">
+        <v>2030919760</v>
+      </c>
+      <c r="H10" t="n">
+        <v>2345674704.76664</v>
+      </c>
+      <c r="I10" t="n">
+        <v>-6953185182.986558</v>
+      </c>
+      <c r="J10" t="n">
+        <v>0</v>
+      </c>
+      <c r="K10" t="n">
+        <v>0</v>
+      </c>
+      <c r="L10" t="n">
+        <v>0</v>
+      </c>
+      <c r="M10" t="n">
+        <v>168992919929.3019</v>
+      </c>
+      <c r="N10" t="n">
+        <v>0</v>
+      </c>
+      <c r="O10" t="n">
+        <v>0</v>
+      </c>
+      <c r="P10" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q10" t="n">
+        <v>0</v>
+      </c>
+      <c r="R10" t="n">
+        <v>0</v>
+      </c>
+      <c r="S10" t="n">
+        <v>0</v>
+      </c>
+      <c r="T10" t="n">
+        <v>0</v>
+      </c>
+      <c r="U10" t="n">
+        <v>0</v>
+      </c>
+      <c r="V10" t="n">
+        <v>734.143000125885</v>
+      </c>
+      <c r="W10" t="n">
+        <v>168992917590.919</v>
+      </c>
+      <c r="X10" t="n">
+        <v>168992919929.3019</v>
+      </c>
+      <c r="Y10" t="n">
+        <v>2338.382965087891</v>
+      </c>
+      <c r="Z10" t="inlineStr">
+        <is>
+          <t>optimal</t>
+        </is>
+      </c>
+      <c r="AA10" t="inlineStr">
+        <is>
+          <t>costs_emissionlimit</t>
+        </is>
+      </c>
+      <c r="AB10" t="n">
+        <v>-1</v>
+      </c>
+      <c r="AC10" t="n">
+        <v>-1</v>
+      </c>
+      <c r="AD10" t="n">
+        <v>1</v>
+      </c>
+      <c r="AE10" t="inlineStr">
+        <is>
+          <t>GreenFieldHydro_NotIsland_2040</t>
+        </is>
+      </c>
+      <c r="AF10" t="inlineStr">
+        <is>
+          <t>rawResults\20260203173001_GreenFieldHydro_NotIsland_2040-1</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Results with export bug fixed
</commit_message>
<xml_diff>
--- a/rawResults/Summary.xlsx
+++ b/rawResults/Summary.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AF14"/>
+  <dimension ref="A1:AF24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1973,6 +1973,1066 @@
         </is>
       </c>
     </row>
+    <row r="15">
+      <c r="A15" t="n">
+        <v>46206429983.8214</v>
+      </c>
+      <c r="B15" t="n">
+        <v>26009944462.88666</v>
+      </c>
+      <c r="C15" t="n">
+        <v>0</v>
+      </c>
+      <c r="D15" t="n">
+        <v>18165565760.93473</v>
+      </c>
+      <c r="E15" t="n">
+        <v>2030919760</v>
+      </c>
+      <c r="F15" t="n">
+        <v>44175510223.8214</v>
+      </c>
+      <c r="G15" t="n">
+        <v>2030919760</v>
+      </c>
+      <c r="H15" t="n">
+        <v>0</v>
+      </c>
+      <c r="I15" t="n">
+        <v>0</v>
+      </c>
+      <c r="J15" t="n">
+        <v>0</v>
+      </c>
+      <c r="K15" t="n">
+        <v>0</v>
+      </c>
+      <c r="L15" t="n">
+        <v>0</v>
+      </c>
+      <c r="M15" t="n">
+        <v>46206429983.8214</v>
+      </c>
+      <c r="N15" t="n">
+        <v>0</v>
+      </c>
+      <c r="O15" t="n">
+        <v>0</v>
+      </c>
+      <c r="P15" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q15" t="n">
+        <v>0</v>
+      </c>
+      <c r="R15" t="n">
+        <v>0</v>
+      </c>
+      <c r="S15" t="n">
+        <v>0</v>
+      </c>
+      <c r="T15" t="n">
+        <v>0</v>
+      </c>
+      <c r="U15" t="n">
+        <v>0</v>
+      </c>
+      <c r="V15" t="n">
+        <v>350.0540001392365</v>
+      </c>
+      <c r="W15" t="n">
+        <v>46206422394.54113</v>
+      </c>
+      <c r="X15" t="n">
+        <v>46206429983.8214</v>
+      </c>
+      <c r="Y15" t="n">
+        <v>7589.280265808105</v>
+      </c>
+      <c r="Z15" t="inlineStr">
+        <is>
+          <t>optimal</t>
+        </is>
+      </c>
+      <c r="AA15" t="inlineStr">
+        <is>
+          <t>costs_emissionlimit</t>
+        </is>
+      </c>
+      <c r="AB15" t="n">
+        <v>-1</v>
+      </c>
+      <c r="AC15" t="n">
+        <v>-1</v>
+      </c>
+      <c r="AD15" t="n">
+        <v>1</v>
+      </c>
+      <c r="AE15" t="inlineStr">
+        <is>
+          <t>Island_lowDisc_greenfield</t>
+        </is>
+      </c>
+      <c r="AF15" t="inlineStr">
+        <is>
+          <t>rawResults\20260215163629_Island_lowDisc_greenfield-1</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="n">
+        <v>69075064785.38065</v>
+      </c>
+      <c r="B16" t="n">
+        <v>49834925167.15388</v>
+      </c>
+      <c r="C16" t="n">
+        <v>0</v>
+      </c>
+      <c r="D16" t="n">
+        <v>17209219858.22677</v>
+      </c>
+      <c r="E16" t="n">
+        <v>2030919760</v>
+      </c>
+      <c r="F16" t="n">
+        <v>67044145025.38065</v>
+      </c>
+      <c r="G16" t="n">
+        <v>2030919760</v>
+      </c>
+      <c r="H16" t="n">
+        <v>0</v>
+      </c>
+      <c r="I16" t="n">
+        <v>0</v>
+      </c>
+      <c r="J16" t="n">
+        <v>0</v>
+      </c>
+      <c r="K16" t="n">
+        <v>0</v>
+      </c>
+      <c r="L16" t="n">
+        <v>0</v>
+      </c>
+      <c r="M16" t="n">
+        <v>69075064785.38065</v>
+      </c>
+      <c r="N16" t="n">
+        <v>0</v>
+      </c>
+      <c r="O16" t="n">
+        <v>0</v>
+      </c>
+      <c r="P16" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q16" t="n">
+        <v>0</v>
+      </c>
+      <c r="R16" t="n">
+        <v>0</v>
+      </c>
+      <c r="S16" t="n">
+        <v>0</v>
+      </c>
+      <c r="T16" t="n">
+        <v>0</v>
+      </c>
+      <c r="U16" t="n">
+        <v>0</v>
+      </c>
+      <c r="V16" t="n">
+        <v>583.933000087738</v>
+      </c>
+      <c r="W16" t="n">
+        <v>69075063524.86021</v>
+      </c>
+      <c r="X16" t="n">
+        <v>69075064785.38065</v>
+      </c>
+      <c r="Y16" t="n">
+        <v>1260.520431518555</v>
+      </c>
+      <c r="Z16" t="inlineStr">
+        <is>
+          <t>optimal</t>
+        </is>
+      </c>
+      <c r="AA16" t="inlineStr">
+        <is>
+          <t>costs_emissionlimit</t>
+        </is>
+      </c>
+      <c r="AB16" t="n">
+        <v>-1</v>
+      </c>
+      <c r="AC16" t="n">
+        <v>-1</v>
+      </c>
+      <c r="AD16" t="n">
+        <v>1</v>
+      </c>
+      <c r="AE16" t="inlineStr">
+        <is>
+          <t>Island_highDisc_greenfield</t>
+        </is>
+      </c>
+      <c r="AF16" t="inlineStr">
+        <is>
+          <t>rawResults\20260215174259_Island_highDisc_greenfield-1</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="n">
+        <v>32379069972.6438</v>
+      </c>
+      <c r="B17" t="n">
+        <v>21203768015.11133</v>
+      </c>
+      <c r="C17" t="n">
+        <v>0</v>
+      </c>
+      <c r="D17" t="n">
+        <v>15672035369.15194</v>
+      </c>
+      <c r="E17" t="n">
+        <v>2030919760</v>
+      </c>
+      <c r="F17" t="n">
+        <v>36875803384.26328</v>
+      </c>
+      <c r="G17" t="n">
+        <v>2030919760</v>
+      </c>
+      <c r="H17" t="n">
+        <v>1393576769.64288</v>
+      </c>
+      <c r="I17" t="n">
+        <v>-7921229941.262362</v>
+      </c>
+      <c r="J17" t="n">
+        <v>0</v>
+      </c>
+      <c r="K17" t="n">
+        <v>0</v>
+      </c>
+      <c r="L17" t="n">
+        <v>0</v>
+      </c>
+      <c r="M17" t="n">
+        <v>32379069972.6438</v>
+      </c>
+      <c r="N17" t="n">
+        <v>0</v>
+      </c>
+      <c r="O17" t="n">
+        <v>0</v>
+      </c>
+      <c r="P17" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q17" t="n">
+        <v>0</v>
+      </c>
+      <c r="R17" t="n">
+        <v>0</v>
+      </c>
+      <c r="S17" t="n">
+        <v>0</v>
+      </c>
+      <c r="T17" t="n">
+        <v>0</v>
+      </c>
+      <c r="U17" t="n">
+        <v>0</v>
+      </c>
+      <c r="V17" t="n">
+        <v>337.835000038147</v>
+      </c>
+      <c r="W17" t="n">
+        <v>32379068444.15659</v>
+      </c>
+      <c r="X17" t="n">
+        <v>32379069972.6438</v>
+      </c>
+      <c r="Y17" t="n">
+        <v>1528.487209320068</v>
+      </c>
+      <c r="Z17" t="inlineStr">
+        <is>
+          <t>optimal</t>
+        </is>
+      </c>
+      <c r="AA17" t="inlineStr">
+        <is>
+          <t>costs_emissionlimit</t>
+        </is>
+      </c>
+      <c r="AB17" t="n">
+        <v>-1</v>
+      </c>
+      <c r="AC17" t="n">
+        <v>-1</v>
+      </c>
+      <c r="AD17" t="n">
+        <v>1</v>
+      </c>
+      <c r="AE17" t="inlineStr">
+        <is>
+          <t>NotIsland_lowDisc_greenfield</t>
+        </is>
+      </c>
+      <c r="AF17" t="inlineStr">
+        <is>
+          <t>rawResults\20260215185359_NotIsland_lowDisc_greenfield-1</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="n">
+        <v>51104080452.09557</v>
+      </c>
+      <c r="B18" t="n">
+        <v>39985471986.5044</v>
+      </c>
+      <c r="C18" t="n">
+        <v>0</v>
+      </c>
+      <c r="D18" t="n">
+        <v>14960541757.22156</v>
+      </c>
+      <c r="E18" t="n">
+        <v>2030919760</v>
+      </c>
+      <c r="F18" t="n">
+        <v>54946013743.72596</v>
+      </c>
+      <c r="G18" t="n">
+        <v>2030919760</v>
+      </c>
+      <c r="H18" t="n">
+        <v>1729431157.270354</v>
+      </c>
+      <c r="I18" t="n">
+        <v>-7602284208.900747</v>
+      </c>
+      <c r="J18" t="n">
+        <v>0</v>
+      </c>
+      <c r="K18" t="n">
+        <v>0</v>
+      </c>
+      <c r="L18" t="n">
+        <v>0</v>
+      </c>
+      <c r="M18" t="n">
+        <v>51104080452.09557</v>
+      </c>
+      <c r="N18" t="n">
+        <v>0</v>
+      </c>
+      <c r="O18" t="n">
+        <v>0</v>
+      </c>
+      <c r="P18" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q18" t="n">
+        <v>0</v>
+      </c>
+      <c r="R18" t="n">
+        <v>0</v>
+      </c>
+      <c r="S18" t="n">
+        <v>0</v>
+      </c>
+      <c r="T18" t="n">
+        <v>0</v>
+      </c>
+      <c r="U18" t="n">
+        <v>0</v>
+      </c>
+      <c r="V18" t="n">
+        <v>999.9100000858307</v>
+      </c>
+      <c r="W18" t="n">
+        <v>51104080209.30309</v>
+      </c>
+      <c r="X18" t="n">
+        <v>51104080452.09557</v>
+      </c>
+      <c r="Y18" t="n">
+        <v>242.79248046875</v>
+      </c>
+      <c r="Z18" t="inlineStr">
+        <is>
+          <t>optimal</t>
+        </is>
+      </c>
+      <c r="AA18" t="inlineStr">
+        <is>
+          <t>costs_emissionlimit</t>
+        </is>
+      </c>
+      <c r="AB18" t="n">
+        <v>-1</v>
+      </c>
+      <c r="AC18" t="n">
+        <v>-1</v>
+      </c>
+      <c r="AD18" t="n">
+        <v>1</v>
+      </c>
+      <c r="AE18" t="inlineStr">
+        <is>
+          <t>NotIsland_highDisc_greenfield</t>
+        </is>
+      </c>
+      <c r="AF18" t="inlineStr">
+        <is>
+          <t>rawResults\20260215200052_NotIsland_highDisc_greenfield-1</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="n">
+        <v>43455224245.01422</v>
+      </c>
+      <c r="B19" t="n">
+        <v>24134714901.498</v>
+      </c>
+      <c r="C19" t="n">
+        <v>0</v>
+      </c>
+      <c r="D19" t="n">
+        <v>17289589583.51621</v>
+      </c>
+      <c r="E19" t="n">
+        <v>2030919760</v>
+      </c>
+      <c r="F19" t="n">
+        <v>41424304485.01422</v>
+      </c>
+      <c r="G19" t="n">
+        <v>2030919760</v>
+      </c>
+      <c r="H19" t="n">
+        <v>0</v>
+      </c>
+      <c r="I19" t="n">
+        <v>0</v>
+      </c>
+      <c r="J19" t="n">
+        <v>0</v>
+      </c>
+      <c r="K19" t="n">
+        <v>0</v>
+      </c>
+      <c r="L19" t="n">
+        <v>0</v>
+      </c>
+      <c r="M19" t="n">
+        <v>43455224245.01422</v>
+      </c>
+      <c r="N19" t="n">
+        <v>0</v>
+      </c>
+      <c r="O19" t="n">
+        <v>0</v>
+      </c>
+      <c r="P19" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q19" t="n">
+        <v>0</v>
+      </c>
+      <c r="R19" t="n">
+        <v>0</v>
+      </c>
+      <c r="S19" t="n">
+        <v>0</v>
+      </c>
+      <c r="T19" t="n">
+        <v>0</v>
+      </c>
+      <c r="U19" t="n">
+        <v>0</v>
+      </c>
+      <c r="V19" t="n">
+        <v>3202.686000108719</v>
+      </c>
+      <c r="W19" t="n">
+        <v>43455223913.79698</v>
+      </c>
+      <c r="X19" t="n">
+        <v>43455224245.01422</v>
+      </c>
+      <c r="Y19" t="n">
+        <v>331.2172393798828</v>
+      </c>
+      <c r="Z19" t="inlineStr">
+        <is>
+          <t>optimal</t>
+        </is>
+      </c>
+      <c r="AA19" t="inlineStr">
+        <is>
+          <t>costs_emissionlimit</t>
+        </is>
+      </c>
+      <c r="AB19" t="n">
+        <v>-1</v>
+      </c>
+      <c r="AC19" t="n">
+        <v>-1</v>
+      </c>
+      <c r="AD19" t="n">
+        <v>1</v>
+      </c>
+      <c r="AE19" t="inlineStr">
+        <is>
+          <t>Island_lowDisc_greenfield</t>
+        </is>
+      </c>
+      <c r="AF19" t="inlineStr">
+        <is>
+          <t>rawResults\20260216121620_Island_lowDisc_greenfield-1</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="n">
+        <v>63105194110.90955</v>
+      </c>
+      <c r="B20" t="n">
+        <v>44263260976.60344</v>
+      </c>
+      <c r="C20" t="n">
+        <v>0</v>
+      </c>
+      <c r="D20" t="n">
+        <v>16811013374.3061</v>
+      </c>
+      <c r="E20" t="n">
+        <v>2030919760</v>
+      </c>
+      <c r="F20" t="n">
+        <v>61074274350.90955</v>
+      </c>
+      <c r="G20" t="n">
+        <v>2030919760</v>
+      </c>
+      <c r="H20" t="n">
+        <v>0</v>
+      </c>
+      <c r="I20" t="n">
+        <v>0</v>
+      </c>
+      <c r="J20" t="n">
+        <v>0</v>
+      </c>
+      <c r="K20" t="n">
+        <v>0</v>
+      </c>
+      <c r="L20" t="n">
+        <v>0</v>
+      </c>
+      <c r="M20" t="n">
+        <v>63105194110.90955</v>
+      </c>
+      <c r="N20" t="n">
+        <v>0</v>
+      </c>
+      <c r="O20" t="n">
+        <v>0</v>
+      </c>
+      <c r="P20" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q20" t="n">
+        <v>0</v>
+      </c>
+      <c r="R20" t="n">
+        <v>0</v>
+      </c>
+      <c r="S20" t="n">
+        <v>0</v>
+      </c>
+      <c r="T20" t="n">
+        <v>0</v>
+      </c>
+      <c r="U20" t="n">
+        <v>0</v>
+      </c>
+      <c r="V20" t="n">
+        <v>4717.499000072479</v>
+      </c>
+      <c r="W20" t="n">
+        <v>63105193966.09333</v>
+      </c>
+      <c r="X20" t="n">
+        <v>63105194110.90955</v>
+      </c>
+      <c r="Y20" t="n">
+        <v>144.8162155151367</v>
+      </c>
+      <c r="Z20" t="inlineStr">
+        <is>
+          <t>optimal</t>
+        </is>
+      </c>
+      <c r="AA20" t="inlineStr">
+        <is>
+          <t>costs_emissionlimit</t>
+        </is>
+      </c>
+      <c r="AB20" t="n">
+        <v>-1</v>
+      </c>
+      <c r="AC20" t="n">
+        <v>-1</v>
+      </c>
+      <c r="AD20" t="n">
+        <v>1</v>
+      </c>
+      <c r="AE20" t="inlineStr">
+        <is>
+          <t>Island_highDisc_greenfield</t>
+        </is>
+      </c>
+      <c r="AF20" t="inlineStr">
+        <is>
+          <t>rawResults\20260216141800_Island_highDisc_greenfield-1</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="n">
+        <v>43455224245.01422</v>
+      </c>
+      <c r="B21" t="n">
+        <v>24134714901.498</v>
+      </c>
+      <c r="C21" t="n">
+        <v>0</v>
+      </c>
+      <c r="D21" t="n">
+        <v>17289589583.51621</v>
+      </c>
+      <c r="E21" t="n">
+        <v>2030919760</v>
+      </c>
+      <c r="F21" t="n">
+        <v>41424304485.01422</v>
+      </c>
+      <c r="G21" t="n">
+        <v>2030919760</v>
+      </c>
+      <c r="H21" t="n">
+        <v>0</v>
+      </c>
+      <c r="I21" t="n">
+        <v>0</v>
+      </c>
+      <c r="J21" t="n">
+        <v>0</v>
+      </c>
+      <c r="K21" t="n">
+        <v>0</v>
+      </c>
+      <c r="L21" t="n">
+        <v>0</v>
+      </c>
+      <c r="M21" t="n">
+        <v>43455224245.01422</v>
+      </c>
+      <c r="N21" t="n">
+        <v>0</v>
+      </c>
+      <c r="O21" t="n">
+        <v>0</v>
+      </c>
+      <c r="P21" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q21" t="n">
+        <v>0</v>
+      </c>
+      <c r="R21" t="n">
+        <v>0</v>
+      </c>
+      <c r="S21" t="n">
+        <v>0</v>
+      </c>
+      <c r="T21" t="n">
+        <v>0</v>
+      </c>
+      <c r="U21" t="n">
+        <v>0</v>
+      </c>
+      <c r="V21" t="n">
+        <v>3123.121000051498</v>
+      </c>
+      <c r="W21" t="n">
+        <v>43455223913.79698</v>
+      </c>
+      <c r="X21" t="n">
+        <v>43455224245.01422</v>
+      </c>
+      <c r="Y21" t="n">
+        <v>331.2172393798828</v>
+      </c>
+      <c r="Z21" t="inlineStr">
+        <is>
+          <t>optimal</t>
+        </is>
+      </c>
+      <c r="AA21" t="inlineStr">
+        <is>
+          <t>costs_emissionlimit</t>
+        </is>
+      </c>
+      <c r="AB21" t="n">
+        <v>-1</v>
+      </c>
+      <c r="AC21" t="n">
+        <v>-1</v>
+      </c>
+      <c r="AD21" t="n">
+        <v>1</v>
+      </c>
+      <c r="AE21" t="inlineStr">
+        <is>
+          <t>Island_lowDisc_greenfield</t>
+        </is>
+      </c>
+      <c r="AF21" t="inlineStr">
+        <is>
+          <t>rawResults\20260216200541_Island_lowDisc_greenfield-1</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="n">
+        <v>63105194110.90955</v>
+      </c>
+      <c r="B22" t="n">
+        <v>44263260976.60344</v>
+      </c>
+      <c r="C22" t="n">
+        <v>0</v>
+      </c>
+      <c r="D22" t="n">
+        <v>16811013374.3061</v>
+      </c>
+      <c r="E22" t="n">
+        <v>2030919760</v>
+      </c>
+      <c r="F22" t="n">
+        <v>61074274350.90955</v>
+      </c>
+      <c r="G22" t="n">
+        <v>2030919760</v>
+      </c>
+      <c r="H22" t="n">
+        <v>0</v>
+      </c>
+      <c r="I22" t="n">
+        <v>0</v>
+      </c>
+      <c r="J22" t="n">
+        <v>0</v>
+      </c>
+      <c r="K22" t="n">
+        <v>0</v>
+      </c>
+      <c r="L22" t="n">
+        <v>0</v>
+      </c>
+      <c r="M22" t="n">
+        <v>63105194110.90955</v>
+      </c>
+      <c r="N22" t="n">
+        <v>0</v>
+      </c>
+      <c r="O22" t="n">
+        <v>0</v>
+      </c>
+      <c r="P22" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q22" t="n">
+        <v>0</v>
+      </c>
+      <c r="R22" t="n">
+        <v>0</v>
+      </c>
+      <c r="S22" t="n">
+        <v>0</v>
+      </c>
+      <c r="T22" t="n">
+        <v>0</v>
+      </c>
+      <c r="U22" t="n">
+        <v>0</v>
+      </c>
+      <c r="V22" t="n">
+        <v>4508.098000049591</v>
+      </c>
+      <c r="W22" t="n">
+        <v>63105193966.09333</v>
+      </c>
+      <c r="X22" t="n">
+        <v>63105194110.90955</v>
+      </c>
+      <c r="Y22" t="n">
+        <v>144.8162155151367</v>
+      </c>
+      <c r="Z22" t="inlineStr">
+        <is>
+          <t>optimal</t>
+        </is>
+      </c>
+      <c r="AA22" t="inlineStr">
+        <is>
+          <t>costs_emissionlimit</t>
+        </is>
+      </c>
+      <c r="AB22" t="n">
+        <v>-1</v>
+      </c>
+      <c r="AC22" t="n">
+        <v>-1</v>
+      </c>
+      <c r="AD22" t="n">
+        <v>1</v>
+      </c>
+      <c r="AE22" t="inlineStr">
+        <is>
+          <t>Island_highDisc_greenfield</t>
+        </is>
+      </c>
+      <c r="AF22" t="inlineStr">
+        <is>
+          <t>rawResults\20260216220706_Island_highDisc_greenfield-1</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="n">
+        <v>37433854532.10802</v>
+      </c>
+      <c r="B23" t="n">
+        <v>19516430826.91516</v>
+      </c>
+      <c r="C23" t="n">
+        <v>0</v>
+      </c>
+      <c r="D23" t="n">
+        <v>14223510095.8617</v>
+      </c>
+      <c r="E23" t="n">
+        <v>2030919760</v>
+      </c>
+      <c r="F23" t="n">
+        <v>33739940922.77686</v>
+      </c>
+      <c r="G23" t="n">
+        <v>2030919760</v>
+      </c>
+      <c r="H23" t="n">
+        <v>1662993849.331164</v>
+      </c>
+      <c r="I23" t="n">
+        <v>0</v>
+      </c>
+      <c r="J23" t="n">
+        <v>0</v>
+      </c>
+      <c r="K23" t="n">
+        <v>0</v>
+      </c>
+      <c r="L23" t="n">
+        <v>0</v>
+      </c>
+      <c r="M23" t="n">
+        <v>37433854532.10802</v>
+      </c>
+      <c r="N23" t="n">
+        <v>0</v>
+      </c>
+      <c r="O23" t="n">
+        <v>0</v>
+      </c>
+      <c r="P23" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q23" t="n">
+        <v>0</v>
+      </c>
+      <c r="R23" t="n">
+        <v>0</v>
+      </c>
+      <c r="S23" t="n">
+        <v>0</v>
+      </c>
+      <c r="T23" t="n">
+        <v>0</v>
+      </c>
+      <c r="U23" t="n">
+        <v>0</v>
+      </c>
+      <c r="V23" t="n">
+        <v>1284.457999944687</v>
+      </c>
+      <c r="W23" t="n">
+        <v>37433853089.32781</v>
+      </c>
+      <c r="X23" t="n">
+        <v>37433854532.10802</v>
+      </c>
+      <c r="Y23" t="n">
+        <v>1442.780212402344</v>
+      </c>
+      <c r="Z23" t="inlineStr">
+        <is>
+          <t>optimal</t>
+        </is>
+      </c>
+      <c r="AA23" t="inlineStr">
+        <is>
+          <t>costs_emissionlimit</t>
+        </is>
+      </c>
+      <c r="AB23" t="n">
+        <v>-1</v>
+      </c>
+      <c r="AC23" t="n">
+        <v>-1</v>
+      </c>
+      <c r="AD23" t="n">
+        <v>1</v>
+      </c>
+      <c r="AE23" t="inlineStr">
+        <is>
+          <t>NotIsland_lowDisc_greenfield</t>
+        </is>
+      </c>
+      <c r="AF23" t="inlineStr">
+        <is>
+          <t>rawResults\20260217003106_NotIsland_lowDisc_greenfield-1</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="n">
+        <v>53036906450.04081</v>
+      </c>
+      <c r="B24" t="n">
+        <v>34764910461.50002</v>
+      </c>
+      <c r="C24" t="n">
+        <v>0</v>
+      </c>
+      <c r="D24" t="n">
+        <v>13789331371.06469</v>
+      </c>
+      <c r="E24" t="n">
+        <v>2030919760</v>
+      </c>
+      <c r="F24" t="n">
+        <v>48554241832.56471</v>
+      </c>
+      <c r="G24" t="n">
+        <v>2030919760</v>
+      </c>
+      <c r="H24" t="n">
+        <v>2451744857.476096</v>
+      </c>
+      <c r="I24" t="n">
+        <v>0</v>
+      </c>
+      <c r="J24" t="n">
+        <v>0</v>
+      </c>
+      <c r="K24" t="n">
+        <v>0</v>
+      </c>
+      <c r="L24" t="n">
+        <v>0</v>
+      </c>
+      <c r="M24" t="n">
+        <v>53036906450.04081</v>
+      </c>
+      <c r="N24" t="n">
+        <v>0</v>
+      </c>
+      <c r="O24" t="n">
+        <v>0</v>
+      </c>
+      <c r="P24" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q24" t="n">
+        <v>0</v>
+      </c>
+      <c r="R24" t="n">
+        <v>0</v>
+      </c>
+      <c r="S24" t="n">
+        <v>0</v>
+      </c>
+      <c r="T24" t="n">
+        <v>0</v>
+      </c>
+      <c r="U24" t="n">
+        <v>0</v>
+      </c>
+      <c r="V24" t="n">
+        <v>2715.637000083923</v>
+      </c>
+      <c r="W24" t="n">
+        <v>53036905992.60873</v>
+      </c>
+      <c r="X24" t="n">
+        <v>53036906450.04081</v>
+      </c>
+      <c r="Y24" t="n">
+        <v>457.4320755004883</v>
+      </c>
+      <c r="Z24" t="inlineStr">
+        <is>
+          <t>optimal</t>
+        </is>
+      </c>
+      <c r="AA24" t="inlineStr">
+        <is>
+          <t>costs_emissionlimit</t>
+        </is>
+      </c>
+      <c r="AB24" t="n">
+        <v>-1</v>
+      </c>
+      <c r="AC24" t="n">
+        <v>-1</v>
+      </c>
+      <c r="AD24" t="n">
+        <v>1</v>
+      </c>
+      <c r="AE24" t="inlineStr">
+        <is>
+          <t>NotIsland_highDisc_greenfield</t>
+        </is>
+      </c>
+      <c r="AF24" t="inlineStr">
+        <is>
+          <t>rawResults\20260217020104_NotIsland_highDisc_greenfield-1</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>